<commit_message>
add more data in overall.xlsx
</commit_message>
<xml_diff>
--- a/data/test/overall.xlsx
+++ b/data/test/overall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\code\ComplexCi\data\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{47E2D23E-81B3-4AA9-AFF6-733F7F5CB27A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9F1CC88A-5993-4872-91DE-8E7E4A9E55FA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="13050" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2174" uniqueCount="832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2168" uniqueCount="827">
   <si>
     <t>model1</t>
   </si>
@@ -2760,51 +2760,31 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>2.94s</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.52s</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>49.26s</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>47.85s</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.84s</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.57s</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>65.74s</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>50.53s</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>PageRank</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>0.07s</t>
+    <t>Trad_CI_l2</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>1.68s</t>
+    <t>Trad_CI_l0</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>1.41s</t>
+    <t>Trad_CI_l1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>New_CI_l0</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>New_CI_l1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>New_CI_l2</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -3082,7 +3062,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3261,9 +3241,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -21545,15 +21522,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E94F2EB7-1E9E-4A39-A4CC-0324EB73E9D6}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.375" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="18.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
@@ -21574,23 +21551,25 @@
       <c r="E1" s="57" t="s">
         <v>819</v>
       </c>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
         <v>817</v>
       </c>
       <c r="B2" s="13">
+        <v>2</v>
+      </c>
+      <c r="C2" s="13">
         <v>3</v>
       </c>
-      <c r="C2" s="13">
-        <v>5</v>
-      </c>
       <c r="D2" s="13">
+        <v>2</v>
+      </c>
+      <c r="E2" s="13">
         <v>3</v>
       </c>
-      <c r="E2" s="13">
-        <v>5</v>
-      </c>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A3" s="13"/>
@@ -21606,7 +21585,7 @@
       <c r="E3" s="2" t="s">
         <v>815</v>
       </c>
-      <c r="F3" s="58"/>
+      <c r="F3" s="2"/>
       <c r="G3" s="58"/>
       <c r="H3" s="58"/>
       <c r="I3" s="58"/>
@@ -21617,19 +21596,19 @@
         <v>794</v>
       </c>
       <c r="B4" s="13">
-        <v>0.29742383321360699</v>
+        <v>0.20010725717615299</v>
       </c>
       <c r="C4" s="13">
-        <v>0.389159047587812</v>
+        <v>0.29474406865075198</v>
       </c>
       <c r="D4" s="13">
-        <v>0.29626129782960497</v>
+        <v>0.19705266981085801</v>
       </c>
       <c r="E4" s="13">
-        <v>0.38742803039496898</v>
-      </c>
-      <c r="F4" s="59">
-        <v>1.37027220902599</v>
+        <v>0.29672736998545801</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0.98863136562322296</v>
       </c>
       <c r="G4" s="59"/>
       <c r="H4" s="59"/>
@@ -21637,102 +21616,191 @@
       <c r="J4" s="59"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A5" s="13"/>
-      <c r="B5" s="57" t="s">
-        <v>824</v>
-      </c>
-      <c r="C5" s="57" t="s">
-        <v>825</v>
-      </c>
-      <c r="D5" s="57" t="s">
-        <v>827</v>
-      </c>
-      <c r="E5" s="57" t="s">
-        <v>826</v>
-      </c>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
+      <c r="A5" s="57" t="s">
+        <v>795</v>
+      </c>
+      <c r="B5" s="13">
+        <v>0.24816608016939701</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0.30359175437149799</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0.25008414853781102</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0.30704661197174499</v>
+      </c>
+      <c r="F5" s="13">
+        <v>1.1088885950504499</v>
+      </c>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
       <c r="J5" s="59"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="57" t="s">
-        <v>795</v>
+        <v>820</v>
       </c>
       <c r="B6" s="13">
-        <v>0.304978248939482</v>
+        <v>0.173950662665741</v>
       </c>
       <c r="C6" s="13">
-        <v>0.38955516034161902</v>
+        <v>0.29617317031817197</v>
       </c>
       <c r="D6" s="13">
-        <v>0.30229781303417802</v>
+        <v>0.173590674992426</v>
       </c>
       <c r="E6" s="13">
-        <v>0.38745130042109999</v>
-      </c>
-      <c r="F6" s="59">
-        <v>1.38428252273638</v>
-      </c>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
+        <v>0.29410477511794197</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0.93781928309428297</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="13"/>
-      <c r="B7" s="57" t="s">
-        <v>820</v>
-      </c>
-      <c r="C7" s="57" t="s">
-        <v>821</v>
-      </c>
-      <c r="D7" s="57" t="s">
-        <v>822</v>
-      </c>
-      <c r="E7" s="57" t="s">
-        <v>823</v>
-      </c>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="59"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A8" s="57" t="s">
-        <v>828</v>
-      </c>
-      <c r="B8" s="13">
-        <v>0.173950662665741</v>
-      </c>
-      <c r="C8" s="13">
-        <v>0.29617317031817197</v>
-      </c>
-      <c r="D8" s="13">
-        <v>0.173590674992426</v>
-      </c>
-      <c r="E8" s="13">
-        <v>0.29410477511794197</v>
-      </c>
-      <c r="F8">
-        <v>0.93781928309428297</v>
-      </c>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="13"/>
-      <c r="B9" s="57" t="s">
-        <v>829</v>
-      </c>
-      <c r="C9" s="57" t="s">
-        <v>829</v>
-      </c>
-      <c r="D9" s="57" t="s">
-        <v>830</v>
-      </c>
-      <c r="E9" s="57" t="s">
-        <v>831</v>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A10" s="57" t="s">
+        <v>822</v>
+      </c>
+      <c r="B10" s="13">
+        <v>6.5356941042468905E-2</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0.132632196192012</v>
+      </c>
+      <c r="D10" s="13">
+        <v>6.2807589401480804E-2</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0.132647919270448</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0.39344464590641098</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A11" s="57" t="s">
+        <v>823</v>
+      </c>
+      <c r="B11" s="13">
+        <v>5.5988551557633999E-2</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0.125198891033448</v>
+      </c>
+      <c r="D11" s="13">
+        <v>5.4240002331090199E-2</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0.12500714500777399</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0.36043458992994698</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A12" s="57" t="s">
+        <v>821</v>
+      </c>
+      <c r="B12" s="13">
+        <v>5.4840245596594103E-2</v>
+      </c>
+      <c r="C12" s="13">
+        <v>0.12479650287299</v>
+      </c>
+      <c r="D12" s="13">
+        <v>5.2341373447429E-2</v>
+      </c>
+      <c r="E12" s="13">
+        <v>0.124643502668765</v>
+      </c>
+      <c r="F12" s="13">
+        <v>0.35662162458577901</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A13" s="57" t="s">
+        <v>824</v>
+      </c>
+      <c r="B13" s="13">
+        <v>4.9231967785871203E-2</v>
+      </c>
+      <c r="C13" s="13">
+        <v>0.123397489563926</v>
+      </c>
+      <c r="D13" s="13">
+        <v>4.79775024889161E-2</v>
+      </c>
+      <c r="E13" s="13">
+        <v>0.123727491213314</v>
+      </c>
+      <c r="F13" s="13">
+        <v>0.34433445105202798</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A14" s="57" t="s">
+        <v>825</v>
+      </c>
+      <c r="B14" s="13">
+        <v>4.8870669900044801E-2</v>
+      </c>
+      <c r="C14" s="13">
+        <v>0.121822565325151</v>
+      </c>
+      <c r="D14" s="13">
+        <v>4.8956955409164601E-2</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0.122397515264221</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0.34204770589858202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A15" s="57" t="s">
+        <v>826</v>
+      </c>
+      <c r="B15" s="13">
+        <v>4.8431827446592697E-2</v>
+      </c>
+      <c r="C15" s="13">
+        <v>0.12136478035046799</v>
+      </c>
+      <c r="D15" s="13">
+        <v>4.7993740363510798E-2</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0.12510573823580901</v>
+      </c>
+      <c r="F15" s="13">
+        <v>0.34289608639638097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>